<commit_message>
Modified Xpath for itdepot.com
</commit_message>
<xml_diff>
--- a/src/main/java/com/test/automation/PcBuild/DataFolder/PriceLists_29-09-2018.xlsx
+++ b/src/main/java/com/test/automation/PcBuild/DataFolder/PriceLists_29-09-2018.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="19">
   <si>
     <t>Company</t>
   </si>
@@ -24,6 +24,51 @@
   </si>
   <si>
     <t>Date</t>
+  </si>
+  <si>
+    <t>TheItDepot</t>
+  </si>
+  <si>
+    <t>AMD Ryzen 5 2600X Processor</t>
+  </si>
+  <si>
+    <t>29/09/2018</t>
+  </si>
+  <si>
+    <t>Asus Prime B350-Plus 7th Gen AMD AM4 Socket Motherboard</t>
+  </si>
+  <si>
+    <t>G.skill Trident Z RGB 16GB (2 x 8GB) DDR4 3200MHz Desktop RAM (F4-3200C16D-16GTZR)</t>
+  </si>
+  <si>
+    <t>Nzxt S340 Elite Tempered Glass Compact ATX Mid-Tower with VR Support - Matte Black</t>
+  </si>
+  <si>
+    <t>Asus Strix Geforce GTX 1060 6GB GDDR5 (STRIX-GTX1060-DC26G)</t>
+  </si>
+  <si>
+    <t>Corsair CX Series CX550 550 Watt 80 Plus Bronze Certified ATX PSU (CP-9020121-UK)</t>
+  </si>
+  <si>
+    <t>MdComputers</t>
+  </si>
+  <si>
+    <t>AMD RYZEN 5 1600 Desktop Processor With Wraith Spire Cooling Solution - (6 Core, Up To 3.6 GHz, AM4 Socket, 19MB Cache)</t>
+  </si>
+  <si>
+    <t>ASUS MOTHERBOARD ROG STRIX B350-F GAMING (AMD SOCKET AM4/RYZEN SERIES CPU/MAX 64GB DDR4-3200MHZ MEMORY)</t>
+  </si>
+  <si>
+    <t>Corsair 16GB DDR4 CMK16GX4M1D3000C16</t>
+  </si>
+  <si>
+    <t>NZXT MID TOWER CABINET (ATX) - SOURCE 340 ELITE WITH TEMPERED GLASS SIDE PANEL (MATTE BLACK)</t>
+  </si>
+  <si>
+    <t>ASUS GRAPHICS CARD PASCAL SERIES - GTX 1060 6GB GDDR5 DC 2 STRIX GAMING EDITION</t>
+  </si>
+  <si>
+    <t>CORSAIR SMPS CX550 - 550 WATT 80 PLUS BRONZE CERTIFICATION PSU WITH ACTIVE PFC</t>
   </si>
 </sst>
 </file>
@@ -68,7 +113,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView tabSelected="true" workbookViewId="0"/>
   </sheetViews>
@@ -87,6 +132,174 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="n">
+        <v>19205.0</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" t="n">
+        <v>12700.0</v>
+      </c>
+      <c r="H2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="n">
+        <v>9940.0</v>
+      </c>
+      <c r="D3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" t="n">
+        <v>11300.0</v>
+      </c>
+      <c r="H3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="n">
+        <v>15240.0</v>
+      </c>
+      <c r="D4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" t="n">
+        <v>12200.0</v>
+      </c>
+      <c r="H4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="n">
+        <v>7775.0</v>
+      </c>
+      <c r="D5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5" t="n">
+        <v>7750.0</v>
+      </c>
+      <c r="H5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" t="n">
+        <v>36185.0</v>
+      </c>
+      <c r="D6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G6" t="n">
+        <v>35000.0</v>
+      </c>
+      <c r="H6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" t="n">
+        <v>4670.0</v>
+      </c>
+      <c r="D7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G7" t="n">
+        <v>4550.0</v>
+      </c>
+      <c r="H7" t="s">
+        <v>6</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>

</xml_diff>

<commit_message>
Changes the product name in config file
</commit_message>
<xml_diff>
--- a/src/main/java/com/test/automation/PcBuild/DataFolder/PriceLists_29-09-2018.xlsx
+++ b/src/main/java/com/test/automation/PcBuild/DataFolder/PriceLists_29-09-2018.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="24">
   <si>
     <t>Company</t>
   </si>
@@ -69,6 +69,21 @@
   </si>
   <si>
     <t>CORSAIR SMPS CX550 - 550 WATT 80 PLUS BRONZE CERTIFICATION PSU WITH ACTIVE PFC</t>
+  </si>
+  <si>
+    <t>PrimeABGB</t>
+  </si>
+  <si>
+    <t>AMD RYZEN 5 2600 6-CORE 3.4 GHZ (3.9 GHZ MAX BOOST) SOCKET AM4 PROCESSOR</t>
+  </si>
+  <si>
+    <t>ASUS ROG STRIX B350-F GAMING AM4 AMD MOTHERBOARD</t>
+  </si>
+  <si>
+    <t>G.SKILL TRIDENTZ RGB 16GB (2 X 8GB) DDR4 DESKTOP RAM F4-3200C14D-16GTZR</t>
+  </si>
+  <si>
+    <t>FRACTAL DESIGN MESHIFY C BLACK CASE FD-CA-MESH-C-BKO-TGL</t>
   </si>
 </sst>
 </file>
@@ -113,7 +128,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView tabSelected="true" workbookViewId="0"/>
   </sheetViews>
@@ -144,6 +159,18 @@
       <c r="H1" t="s">
         <v>3</v>
       </c>
+      <c r="I1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K1" t="s">
+        <v>2</v>
+      </c>
+      <c r="L1" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
@@ -170,6 +197,18 @@
       <c r="H2" t="s">
         <v>6</v>
       </c>
+      <c r="I2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K2" t="n">
+        <v>17344.0</v>
+      </c>
+      <c r="L2" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
@@ -196,6 +235,18 @@
       <c r="H3" t="s">
         <v>6</v>
       </c>
+      <c r="I3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J3" t="s">
+        <v>21</v>
+      </c>
+      <c r="K3" t="n">
+        <v>11275.0</v>
+      </c>
+      <c r="L3" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
@@ -222,6 +273,18 @@
       <c r="H4" t="s">
         <v>6</v>
       </c>
+      <c r="I4" t="s">
+        <v>19</v>
+      </c>
+      <c r="J4" t="s">
+        <v>22</v>
+      </c>
+      <c r="K4" t="n">
+        <v>22524.0</v>
+      </c>
+      <c r="L4" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
@@ -246,6 +309,18 @@
         <v>7750.0</v>
       </c>
       <c r="H5" t="s">
+        <v>6</v>
+      </c>
+      <c r="I5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J5" t="s">
+        <v>23</v>
+      </c>
+      <c r="K5" t="n">
+        <v>9189.0</v>
+      </c>
+      <c r="L5" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>